<commit_message>
updated github pages with new code
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-tr-general-codes-cs.xlsx
+++ b/docs/CodeSystem-tr-general-codes-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
   <si>
     <t>Property</t>
   </si>
@@ -117,7 +117,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>12</t>
+    <t>17</t>
   </si>
   <si>
     <t>Level</t>
@@ -225,6 +225,24 @@
     <t>Breathing Assessment</t>
   </si>
   <si>
+    <t>brf</t>
+  </si>
+  <si>
+    <t>Breathing Finding</t>
+  </si>
+  <si>
+    <t>Breahting Finding Section</t>
+  </si>
+  <si>
+    <t>brp</t>
+  </si>
+  <si>
+    <t>Breathing Procedure</t>
+  </si>
+  <si>
+    <t>Breathing Procedure Section</t>
+  </si>
+  <si>
     <t>cir</t>
   </si>
   <si>
@@ -234,6 +252,18 @@
     <t>Circulation Assessment</t>
   </si>
   <si>
+    <t>cirob</t>
+  </si>
+  <si>
+    <t>Circulation Observation</t>
+  </si>
+  <si>
+    <t>cirpro</t>
+  </si>
+  <si>
+    <t>Circulation Procedure</t>
+  </si>
+  <si>
     <t>dis</t>
   </si>
   <si>
@@ -241,6 +271,15 @@
   </si>
   <si>
     <t>Disability Assessment</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>Exposure</t>
+  </si>
+  <si>
+    <t>Exposure Assessment</t>
   </si>
 </sst>
 </file>
@@ -549,7 +588,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -737,6 +776,76 @@
         <v>75</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s" s="2">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>